<commit_message>
Uber Q2 2022 results
</commit_message>
<xml_diff>
--- a/rlang/uber-profit-loss.xlsx
+++ b/rlang/uber-profit-loss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sleet\src\ridehail\rlang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE078644-A88F-4D7C-92B5-5AF37D74D3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14FFD4C-0A1C-40D3-B526-55A3F17FA2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{57121A93-DE6B-494A-9DED-4B862E3AC3F6}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{57121A93-DE6B-494A-9DED-4B862E3AC3F6}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;L" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,21 @@
     <author>Tom Slee</author>
   </authors>
   <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00ED708A-B528-4BAA-8BE6-36F3A28E3AC3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tom Slee: Mobility revenue/ gross bookings
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E10" authorId="0" shapeId="0" xr:uid="{68FB9135-3929-4CDF-8568-AC77D5861D64}">
       <text>
         <r>
@@ -252,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>Profit / Loss ($B)</t>
   </si>
@@ -447,6 +462,9 @@
   </si>
   <si>
     <t>Computed take rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://investor.uber.com/news-events/news/press-release-details/2022/Uber-Announces-Results-for-Second-Quarter-2022/default.aspx </t>
   </si>
 </sst>
 </file>
@@ -567,13 +585,12 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -596,7 +613,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
@@ -689,16 +706,13 @@
           </a:p>
           <a:p>
             <a:pPr algn="l">
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2000">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="85000"/>
                     <a:lumOff val="15000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -801,6 +815,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1006,6 +1021,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.5529999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1242,6 +1260,9 @@
                 <c:pt idx="28">
                   <c:v>-5.9</c:v>
                 </c:pt>
+                <c:pt idx="29">
+                  <c:v>-2.601</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1271,6 +1292,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1448,6 +1470,9 @@
                 <c:pt idx="28">
                   <c:v>1.72</c:v>
                 </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.8720000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1475,8 +1500,11 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1490,7 +1518,9 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1564,6 +1594,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0.16800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.36399999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1586,6 +1619,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1661,6 +1695,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>-0.48199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.71299999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1884,7 +1921,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.12314694302918018"/>
           <c:y val="7.3818977495967164E-2"/>
-          <c:w val="8.0207650414178683E-2"/>
+          <c:w val="0.24732048733962947"/>
           <c:h val="0.16795619017367905"/>
         </c:manualLayout>
       </c:layout>
@@ -2515,7 +2552,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{82200E4A-E82C-4274-9E48-1F87C10FBE87}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0"/>
+    <sheetView zoomScale="200" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2526,7 +2563,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659091" cy="6286500"/>
+    <xdr:ext cx="2887870" cy="2095500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2854,18 +2891,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D3D3FC-8B99-4752-A7B2-3B559B0FE7B5}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="2" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="20" customWidth="1"/>
-    <col min="5" max="6" width="18" style="20" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="19" customWidth="1"/>
+    <col min="5" max="6" width="18" style="19" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="13" width="14.140625" hidden="1" customWidth="1"/>
@@ -2873,50 +2910,50 @@
     <col min="15" max="15" width="114.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2928,16 +2965,16 @@
         <f>CONCATENATE(YEAR(A2), "-", ROUNDUP(MONTH(A2)/3,0))</f>
         <v>2015-1</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="21">
         <v>0.25</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="23">
         <v>-0.2</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -2948,16 +2985,16 @@
         <f t="shared" ref="B3:B33" si="0">CONCATENATE(YEAR(A3), "-", ROUNDUP(MONTH(A3)/3,0))</f>
         <v>2015-2</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>0.35</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -2968,16 +3005,16 @@
         <f t="shared" si="0"/>
         <v>2015-3</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <v>0.7</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>-0.65</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -2988,16 +3025,16 @@
         <f t="shared" si="0"/>
         <v>2015-4</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>0.8</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
       <c r="K5">
         <v>1999</v>
       </c>
@@ -3017,16 +3054,16 @@
         <f t="shared" si="0"/>
         <v>2016-1</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>0.95</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>-0.5</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
       <c r="M6" t="s">
         <v>62</v>
       </c>
@@ -3040,17 +3077,17 @@
         <f t="shared" si="0"/>
         <v>2016-2</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="23">
         <v>-0.75</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="25"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -3061,17 +3098,17 @@
         <f t="shared" si="0"/>
         <v>2016-3</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="21">
         <v>1.7</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <v>-0.9</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="25"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -3082,17 +3119,17 @@
         <f t="shared" si="0"/>
         <v>2016-4</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <v>2.8</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="23">
         <v>-0.99099999999999999</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="25">
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="24">
         <v>2000</v>
       </c>
       <c r="L9">
@@ -3108,19 +3145,19 @@
         <f t="shared" si="0"/>
         <v>2017-1</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="21">
         <v>3.4</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="23">
         <v>-0.70799999999999996</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="23">
         <v>-0.65700000000000003</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="25"/>
+      <c r="F10" s="23"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="24"/>
       <c r="M10" t="s">
         <v>1</v>
       </c>
@@ -3140,23 +3177,23 @@
         <f t="shared" si="0"/>
         <v>2017-2</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="21">
         <v>1.75</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="23">
         <v>-0.64500000000000002</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="23">
         <f>-0.688</f>
         <v>-0.68799999999999994</v>
       </c>
-      <c r="F11" s="24"/>
+      <c r="F11" s="23"/>
       <c r="H11">
         <v>0.88900000000000001</v>
       </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="25"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="24"/>
       <c r="N11" s="3" t="s">
         <v>20</v>
       </c>
@@ -3170,25 +3207,25 @@
         <f t="shared" si="0"/>
         <v>2017-3</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="21">
         <v>2.0099999999999998</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="23">
         <v>-1.5</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="23">
         <v>-0.73599999999999999</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" s="23"/>
       <c r="G12">
         <v>-0.74299999999999999</v>
       </c>
       <c r="H12">
         <v>0.98499999999999999</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="25"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="24"/>
       <c r="N12" s="3" t="s">
         <v>14</v>
       </c>
@@ -3202,22 +3239,22 @@
         <f t="shared" si="0"/>
         <v>2017-4</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="21">
         <v>2.2599999999999998</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="23">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="23">
         <v>-0.56100000000000005</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="23"/>
       <c r="H13">
         <v>1.0880000000000001</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="26">
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="25">
         <v>2001</v>
       </c>
       <c r="L13">
@@ -3242,16 +3279,16 @@
         <f t="shared" si="0"/>
         <v>2018-1</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="21">
         <v>2.5</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <v>-0.57699999999999996</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="23">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="23">
         <v>-0.47799999999999998</v>
       </c>
       <c r="G14">
@@ -3260,12 +3297,12 @@
       <c r="H14">
         <v>1.1359999999999999</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="26">
         <f>2584/10893</f>
         <v>0.23721656109428074</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="25"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="24"/>
       <c r="M14" t="s">
         <v>22</v>
       </c>
@@ -3282,16 +3319,16 @@
         <f t="shared" si="0"/>
         <v>2018-2</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="21">
         <v>2.7</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <v>-0.63800000000000001</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="23">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="23">
         <v>-0.73899999999999999</v>
       </c>
       <c r="G15">
@@ -3300,12 +3337,12 @@
       <c r="H15">
         <v>1.242</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="26">
         <f>2768/12012</f>
         <v>0.23043623043623043</v>
       </c>
-      <c r="J15" s="27"/>
-      <c r="K15" s="25"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="24"/>
       <c r="N15" s="3" t="s">
         <v>2</v>
       </c>
@@ -3319,16 +3356,16 @@
         <f t="shared" si="0"/>
         <v>2018-3</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="21">
         <v>2.95</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <v>-0.93899999999999995</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="23">
         <v>-0.45800000000000002</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="23">
         <v>-0.76300000000000001</v>
       </c>
       <c r="G16">
@@ -3337,12 +3374,12 @@
       <c r="H16">
         <v>1.3480000000000001</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="26">
         <f>2425/10488</f>
         <v>0.23121662852784133</v>
       </c>
-      <c r="J16" s="27"/>
-      <c r="K16" s="25"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="24"/>
       <c r="N16" s="3" t="s">
         <v>41</v>
       </c>
@@ -3356,16 +3393,16 @@
         <f t="shared" si="0"/>
         <v>2018-4</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="21">
         <v>3</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="23">
         <v>-0.37</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="23">
         <v>-0.81699999999999995</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="23">
         <v>-1.0529999999999999</v>
       </c>
       <c r="G17">
@@ -3374,12 +3411,12 @@
       <c r="H17">
         <v>1.4930000000000001</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="26">
         <f>2400/11479</f>
         <v>0.2090774457705375</v>
       </c>
-      <c r="J17" s="27"/>
-      <c r="K17" s="26">
+      <c r="J17" s="26"/>
+      <c r="K17" s="25">
         <v>2002</v>
       </c>
       <c r="L17">
@@ -3398,27 +3435,27 @@
         <f t="shared" si="0"/>
         <v>2019-1</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="21">
         <v>3.1</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="23">
         <v>-1.01</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="23">
         <v>-0.86899999999999999</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="23">
         <v>-1.034</v>
       </c>
       <c r="H18">
         <v>1.55</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="26">
         <f>3099/14649</f>
         <v>0.21155027646938357</v>
       </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="25"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="24"/>
       <c r="N18" s="3" t="s">
         <v>4</v>
       </c>
@@ -3435,27 +3472,27 @@
         <f t="shared" si="0"/>
         <v>2019-2</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="21">
         <v>3.17</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="23">
         <v>-5.2</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="23">
         <v>-0.65600000000000003</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="23">
         <v>-5.4850000000000003</v>
       </c>
       <c r="H19">
         <v>1.677</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="26">
         <f>3166/15756</f>
         <v>0.20093932470170095</v>
       </c>
-      <c r="J19" s="27"/>
-      <c r="K19" s="25"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="24"/>
       <c r="M19" s="1" t="s">
         <v>59</v>
       </c>
@@ -3475,27 +3512,27 @@
         <f t="shared" si="0"/>
         <v>2019-3</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="21">
         <v>3.81</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="23">
         <v>-1.1599999999999999</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="23">
         <v>-0.58499999999999996</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="23">
         <v>-1.1060000000000001</v>
       </c>
       <c r="H20">
         <v>1.77</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="26">
         <f>2895/12554</f>
         <v>0.23060379162020073</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="25"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="24"/>
       <c r="N20" s="3" t="s">
         <v>6</v>
       </c>
@@ -3512,27 +3549,27 @@
         <f t="shared" si="0"/>
         <v>2019-4</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="21">
         <v>4.04</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="23">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="23">
         <v>-0.61499999999999999</v>
       </c>
-      <c r="F21" s="24">
+      <c r="F21" s="23">
         <v>-0.97099999999999997</v>
       </c>
       <c r="H21">
         <v>1.907</v>
       </c>
-      <c r="I21" s="27">
+      <c r="I21" s="26">
         <f>3056/13512</f>
         <v>0.22616933096506808</v>
       </c>
-      <c r="J21" s="27"/>
-      <c r="K21" s="26">
+      <c r="J21" s="26"/>
+      <c r="K21" s="25">
         <v>2003</v>
       </c>
       <c r="L21">
@@ -3554,29 +3591,29 @@
         <f t="shared" si="0"/>
         <v>2020-1</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="21">
         <v>2.4670000000000001</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="23">
         <v>-2.9359999999999999</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="23">
         <v>-0.61199999999999999</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="23">
         <v>-1.2629999999999999</v>
       </c>
       <c r="H22">
         <v>1.6579999999999999</v>
       </c>
-      <c r="I22" s="27">
+      <c r="I22" s="26">
         <f>2467/10874</f>
         <v>0.22687143645392679</v>
       </c>
-      <c r="J22" s="27">
+      <c r="J22" s="26">
         <v>0.22700000000000001</v>
       </c>
-      <c r="K22" s="25"/>
+      <c r="K22" s="24"/>
       <c r="N22" s="3" t="s">
         <v>8</v>
       </c>
@@ -3593,29 +3630,29 @@
         <f t="shared" si="0"/>
         <v>2020-2</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="21">
         <v>0.78700000000000003</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="23">
         <v>-1.7749999999999999</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="23">
         <v>-0.83699999999999997</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="23">
         <v>-1.607</v>
       </c>
       <c r="H23">
         <v>0.73699999999999999</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I23" s="26">
         <f>787/3046</f>
         <v>0.25837163493105714</v>
       </c>
-      <c r="J23" s="27">
+      <c r="J23" s="26">
         <v>0.25800000000000001</v>
       </c>
-      <c r="K23" s="25"/>
+      <c r="K23" s="24"/>
       <c r="N23" s="3" t="s">
         <v>9</v>
       </c>
@@ -3632,29 +3669,29 @@
         <f t="shared" si="0"/>
         <v>2020-3</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="21">
         <v>1.3640000000000001</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="23">
         <v>-1.0900000000000001</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="23">
         <v>-0.625</v>
       </c>
-      <c r="F24" s="24">
+      <c r="F24" s="23">
         <v>-1.1160000000000001</v>
       </c>
       <c r="H24">
         <v>1.1839999999999999</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="26">
         <f>1364/5905</f>
         <v>0.23099068585944116</v>
       </c>
-      <c r="J24" s="27">
+      <c r="J24" s="26">
         <v>0.23100000000000001</v>
       </c>
-      <c r="K24" s="25"/>
+      <c r="K24" s="24"/>
       <c r="N24" s="3" t="s">
         <v>10</v>
       </c>
@@ -3670,29 +3707,29 @@
         <f t="shared" si="0"/>
         <v>2020-4</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="21">
         <v>1.4710000000000001</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="23">
         <v>-0.96799999999999997</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="23">
         <v>-0.45400000000000001</v>
       </c>
-      <c r="F25" s="24">
+      <c r="F25" s="23">
         <v>-0.877</v>
       </c>
       <c r="H25">
         <v>1.4430000000000001</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I25" s="26">
         <f>1.471/6.789</f>
         <v>0.21667403152157905</v>
       </c>
-      <c r="J25" s="27">
+      <c r="J25" s="26">
         <v>0.217</v>
       </c>
-      <c r="K25" s="26">
+      <c r="K25" s="25">
         <v>2004</v>
       </c>
       <c r="L25">
@@ -3713,30 +3750,30 @@
         <f t="shared" si="0"/>
         <v>2021-1</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="21">
         <v>0.85299999999999998</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="23">
         <v>-0.108</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="23">
         <v>-0.35899999999999999</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="23">
         <v>-1.524</v>
       </c>
       <c r="H26">
         <v>1.4470000000000001</v>
       </c>
-      <c r="I26" s="27">
+      <c r="I26" s="26">
         <f>853/6773</f>
         <v>0.12594123726561346</v>
       </c>
-      <c r="J26" s="27">
+      <c r="J26" s="26">
         <v>0.126</v>
       </c>
-      <c r="K26" s="25"/>
-      <c r="M26" s="15" t="s">
+      <c r="K26" s="24"/>
+      <c r="M26" s="14" t="s">
         <v>37</v>
       </c>
       <c r="N26" s="3" t="s">
@@ -3754,29 +3791,29 @@
         <f t="shared" si="0"/>
         <v>2021-2</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="21">
         <v>1.6180000000000001</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="23">
         <v>1.1439999999999999</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="23">
         <v>-0.50900000000000001</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="23">
         <v>-1.1879999999999999</v>
       </c>
       <c r="H27">
         <v>1.5109999999999999</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="26">
         <f>1618/8640</f>
         <v>0.18726851851851853</v>
       </c>
-      <c r="J27" s="27">
+      <c r="J27" s="26">
         <v>0.187</v>
       </c>
-      <c r="K27" s="25"/>
+      <c r="K27" s="24"/>
       <c r="M27" t="s">
         <v>39</v>
       </c>
@@ -3795,29 +3832,29 @@
         <f t="shared" si="0"/>
         <v>2021-3</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="21">
         <v>2.2050000000000001</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="23">
         <v>-2.4</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28" s="23">
         <v>-0.57199999999999995</v>
       </c>
       <c r="H28">
         <v>1.641</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="26">
         <f>2205/9883</f>
         <v>0.22311039158150359</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J28" s="26">
         <v>0.223</v>
       </c>
-      <c r="K28" s="25"/>
+      <c r="K28" s="24"/>
       <c r="M28" t="s">
         <v>40</v>
       </c>
@@ -3836,29 +3873,29 @@
         <f t="shared" si="0"/>
         <v>2021-4</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="21">
         <v>2.278</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="23">
         <v>0.89</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="23">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="23">
         <v>-0.55000000000000004</v>
       </c>
       <c r="H29">
         <v>1.77</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="26">
         <f>2.278/11.34</f>
         <v>0.20088183421516756</v>
       </c>
-      <c r="J29" s="27">
+      <c r="J29" s="26">
         <v>0.20100000000000001</v>
       </c>
-      <c r="K29" s="26">
+      <c r="K29" s="25">
         <v>2005</v>
       </c>
       <c r="L29">
@@ -3879,26 +3916,26 @@
         <f t="shared" si="0"/>
         <v>2022-1</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="21">
         <v>2.52</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="23">
         <v>-5.9</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="23">
         <v>0.16800000000000001</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="23">
         <v>-0.48199999999999998</v>
       </c>
       <c r="H30">
         <v>1.72</v>
       </c>
-      <c r="I30" s="27">
+      <c r="I30" s="26">
         <f>2518/10723</f>
         <v>0.23482234449314557</v>
       </c>
-      <c r="J30" s="27">
+      <c r="J30" s="26">
         <v>0.23499999999999999</v>
       </c>
       <c r="N30" t="s">
@@ -3915,6 +3952,31 @@
       <c r="B31" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2022-2</v>
+      </c>
+      <c r="C31" s="21">
+        <v>3.5529999999999999</v>
+      </c>
+      <c r="D31" s="23">
+        <v>-2.601</v>
+      </c>
+      <c r="E31" s="23">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="F31" s="23">
+        <v>-0.71299999999999997</v>
+      </c>
+      <c r="H31">
+        <v>1.8720000000000001</v>
+      </c>
+      <c r="I31" s="26">
+        <f>3553/13364</f>
+        <v>0.26586351391798863</v>
+      </c>
+      <c r="J31" s="26">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3959,9 +4021,10 @@
     <hyperlink ref="N29" r:id="rId20" xr:uid="{B79A578C-9558-49CA-9095-698179928FCB}"/>
     <hyperlink ref="O30" r:id="rId21" xr:uid="{C705DCCF-249A-49FC-A1B0-052F4469FFE9}"/>
     <hyperlink ref="O22" r:id="rId22" xr:uid="{9DDCE714-50C1-4F1F-80A8-95D19971AAA5}"/>
+    <hyperlink ref="O31" r:id="rId23" xr:uid="{75AD9778-FABD-4C70-A8A8-C8FFA47D8D2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId23"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
 
@@ -3976,97 +4039,97 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>8.6999999999999993</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>1.75</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="7">
+      <c r="D7" s="8"/>
+      <c r="E7" s="6">
         <v>645</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>7.5</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>1.5</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>3.4</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>708</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>6.9</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0.8</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>2.9</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>991</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>5.4</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10">
         <v>1.66</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>934</v>
       </c>
     </row>
@@ -4074,13 +4137,13 @@
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4112,7 +4175,7 @@
         <f t="shared" si="0"/>
         <v>2017-1</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="13">
         <v>6.9359999999999999</v>
       </c>
     </row>
@@ -4125,7 +4188,7 @@
         <f t="shared" si="0"/>
         <v>2017-2</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <v>8.0719999999999992</v>
       </c>
     </row>
@@ -4138,7 +4201,7 @@
         <f t="shared" si="0"/>
         <v>2017-3</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <v>9.0239999999999991</v>
       </c>
     </row>
@@ -4151,7 +4214,7 @@
         <f t="shared" si="0"/>
         <v>2017-4</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="13">
         <v>10.31</v>
       </c>
     </row>
@@ -4164,7 +4227,7 @@
         <f t="shared" si="0"/>
         <v>2018-1</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="13">
         <v>10.853</v>
       </c>
     </row>
@@ -4177,7 +4240,7 @@
         <f t="shared" si="0"/>
         <v>2018-2</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="13">
         <v>11.94</v>
       </c>
     </row>
@@ -4190,7 +4253,7 @@
         <f t="shared" si="0"/>
         <v>2018-3</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <v>12.599</v>
       </c>
     </row>
@@ -4203,7 +4266,7 @@
         <f t="shared" si="0"/>
         <v>2018-4</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="13">
         <v>14.04</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New plots in R project
</commit_message>
<xml_diff>
--- a/rlang/uber-profit-loss.xlsx
+++ b/rlang/uber-profit-loss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sleet\src\ridehail\rlang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14FFD4C-0A1C-40D3-B526-55A3F17FA2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8B359F-6EA4-447A-9A1A-250C015672A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{57121A93-DE6B-494A-9DED-4B862E3AC3F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{57121A93-DE6B-494A-9DED-4B862E3AC3F6}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;L" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,31 @@
     <author>Tom Slee</author>
   </authors>
   <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{D2E3238C-CBE3-4AA4-9977-7244B3F92257}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tom Slee: consolidated statement of operatinos
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+From the Condensed Consolidated Statement of Operations in Supplementary material</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00ED708A-B528-4BAA-8BE6-36F3A28E3AC3}">
       <text>
         <r>
@@ -2552,7 +2577,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{82200E4A-E82C-4274-9E48-1F87C10FBE87}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2563,7 +2588,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2887870" cy="2095500"/>
+    <xdr:ext cx="8667750" cy="6291263"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2891,9 +2916,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D3D3FC-8B99-4752-A7B2-3B559B0FE7B5}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O32" sqref="O32"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>